<commit_message>
[FEATURE] Updated the data prep pipeline with final dataset and some corrections
</commit_message>
<xml_diff>
--- a/final_categ_ads_products_data.xlsx
+++ b/final_categ_ads_products_data.xlsx
@@ -483,8 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>**Winter Wonderland Sale**	Dec 01 – Dec 15
-Embrace the chill with our Winter Wonderland Sale! Wrap yourself in style with the Luxe Cloudspire Winter Wrap Coat or the Luxe Cozy Autumn Cardigan. Enjoy a warm discount of up to 20% off on selected items. Don’t miss this chance to elevate your winter wardrobe! Shop now!</t>
+          <t>**Winter Wonderland Sale**\tDec 01 – Dec 15\nEmbrace the chill with our Winter Wonderland Sale! Wrap yourself in style with the Luxe Cloudspire Winter Wrap Coat or the Luxe Cozy Autumn Cardigan. Enjoy a warm discount of up to 20% off on selected items. Don’t miss this chance to elevate your winter wardrobe! Shop now!</t>
         </is>
       </c>
     </row>
@@ -511,8 +510,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>**Festive Fashion Frenzy**	Dec 16 – Dec 26
-Celebrate the season with our Festive Fashion Frenzy! Discover the LuxeWinter Raindrop Shield Jacket and the LuxeSunny Winter Wool Wrap for cozy gatherings. Get up to 25% off on holiday essentials. Sparkle in style this festive season! Limited time offer!</t>
+          <t>**Festive Fashion Frenzy**\tDec 16 – Dec 26\nCelebrate the season with our Festive Fashion Frenzy! Discover the LuxeWinter Raindrop Shield Jacket and the LuxeSunny Winter Wool Wrap for cozy gatherings. Get up to 25% off on holiday essentials. Sparkle in style this festive season! Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -539,8 +537,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>**New Year, New Wardrobe**	Dec 27 – Jan 10
-Kickstart the New Year with a fresh wardrobe! Upgrade your style with the LuxeBreeze Sunlit Summer Tunic and Luxe AutumnCloud Cashmere Wrap. Enjoy up to 30% off on selected styles. Make 2024 your most fashionable year yet! Shop now!</t>
+          <t>**New Year, New Wardrobe**\tDec 27 – Jan 10\nKickstart the New Year with a fresh wardrobe! Upgrade your style with the LuxeBreeze Sunlit Summer Tunic and Luxe AutumnCloud Cashmere Wrap. Enjoy up to 30% off on selected styles. Make 2024 your most fashionable year yet! Shop now!</t>
         </is>
       </c>
     </row>
@@ -567,8 +564,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>**Cozy Comforts Collection**	Jan 11 – Jan 25
-Dive into the Cozy Comforts Collection! Snuggle up in our SnowSprout Luxe Fleece Pullover or the LuxeRain Classic Trench Overcoat. Enjoy a delightful 15% off your favorite winter staples. Wrap yourself in warmth today!</t>
+          <t>**Cozy Comforts Collection**\tJan 11 – Jan 25\nDive into the Cozy Comforts Collection! Snuggle up in our SnowSprout Luxe Fleece Pullover or the LuxeRain Classic Trench Overcoat. Enjoy a delightful 15% off your favorite winter staples. Wrap yourself in warmth today!</t>
         </is>
       </c>
     </row>
@@ -595,8 +591,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>**Spring Refresh Sale**	Feb 01 – Feb 14
-Welcome spring with open arms! Refresh your wardrobe with the LuxeSpring Eco Linen Wrap Dress and the LuxeCloud Breezy Summer Tunic. Enjoy up to 20% off on select spring arrivals. Step into the new season in style! Shop now!</t>
+          <t>**Spring Refresh Sale**\tFeb 01 – Feb 14\nWelcome spring with open arms! Refresh your wardrobe with the LuxeSpring Eco Linen Wrap Dress and the LuxeCloud Breezy Summer Tunic. Enjoy up to 20% off on select spring arrivals. Step into the new season in style! Shop now!</t>
         </is>
       </c>
     </row>
@@ -623,8 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>**Valentine's Day Love**	Feb 15 – Feb 28
-Spread the love this Valentine’s Day! Gift yourself or a loved one the Luxe AutumnWrap Scarf or the Luxe Cozy Autumn Cardigan. Enjoy a sweet deal of Buy 2 Get 1 Free on selected items. Love is in the air—don’t miss out!</t>
+          <t>**Valentine's Day Love**\tFeb 15 – Feb 28\nSpread the love this Valentine’s Day! Gift yourself or a loved one the Luxe AutumnWrap Scarf or the Luxe Cozy Autumn Cardigan. Enjoy a sweet deal of Buy 2 Get 1 Free on selected items. Love is in the air—don’t miss out!</t>
         </is>
       </c>
     </row>
@@ -651,8 +645,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>**March into Spring Savings**	Mar 01 – Mar 15
-March into savings with our Spring Sale! Brighten up your closet with the Luxe CloudVista Breezy Tunic and LuxeRain Classic Trench Overcoat. Enjoy up to 25% off on selected spring styles. Refresh your wardrobe today!</t>
+          <t>**March into Spring Savings**\tMar 01 – Mar 15\nMarch into savings with our Spring Sale! Brighten up your closet with the Luxe CloudVista Breezy Tunic and LuxeRain Classic Trench Overcoat. Enjoy up to 25% off on selected spring styles. Refresh your wardrobe today!</t>
         </is>
       </c>
     </row>
@@ -679,8 +672,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>**Earth Day Eco	Friendly Sale** – Apr 15 – Apr 30
-Celebrate Earth Day with sustainable fashion! Explore our LuxeSpring Eco Linen Wrap Dress and enjoy up to 30% off on eco-friendly styles. Dress beautifully while caring for our planet. Shop sustainably!</t>
+          <t>**Earth Day Eco\tFriendly Sale** – Apr 15 – Apr 30\nCelebrate Earth Day with sustainable fashion! Explore our LuxeSpring Eco Linen Wrap Dress and enjoy up to 30% off on eco-friendly styles. Dress beautifully while caring for our planet. Shop sustainably!</t>
         </is>
       </c>
     </row>
@@ -707,8 +699,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>**Summer Kick	Off Event** – May 01 – May 15
-Get ready for the sun! Kick off summer with the LuxeBreeze Sunlit Summer Tunic and LuxeCloud Breezy Summer Tunic. Enjoy a bright 20% off on select summer styles. Let your summer style shine! Limited time offer!</t>
+          <t>**Summer Kick\tOff Event** – May 01 – May 15\nGet ready for the sun! Kick off summer with the LuxeBreeze Sunlit Summer Tunic and LuxeCloud Breezy Summer Tunic. Enjoy a bright 20% off on select summer styles. Let your summer style shine! Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -735,8 +726,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>**Monsoon Ready Collection**	Jun 01 – Jun 15
-Be prepared for the rains with our Monsoon Ready Collection! Stay dry and stylish in the RainGuard Luxe Spring Waterproof Jacket and Luxe Rain Classic Trench Overcoat. Enjoy up to 15% off on rain-ready fashion. Stay fashionable through the storms!</t>
+          <t>**Monsoon Ready Collection**\tJun 01 – Jun 15\nBe prepared for the rains with our Monsoon Ready Collection! Stay dry and stylish in the RainGuard Luxe Spring Waterproof Jacket and Luxe Rain Classic Trench Overcoat. Enjoy up to 15% off on rain-ready fashion. Stay fashionable through the storms!</t>
         </is>
       </c>
     </row>
@@ -763,8 +753,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>**Back to School Style**	Jul 01 – Jul 15
-Gear up for a stylish school year! Discover comfy and chic options like the SnowGuard Luxe Thermal Coat and Luxe Cozy Autumn Cardigan. Enjoy up to 20% off on back-to-school essentials. Get ready to learn in style!</t>
+          <t>**Back to School Style**\tJul 01 – Jul 15\nGear up for a stylish school year! Discover comfy and chic options like the SnowGuard Luxe Thermal Coat and Luxe Cozy Autumn Cardigan. Enjoy up to 20% off on back-to-school essentials. Get ready to learn in style!</t>
         </is>
       </c>
     </row>
@@ -791,8 +780,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>**Fall Fashion Fest**	Oct 01 – Oct 15
-Celebrate the beauty of autumn with our Fall Fashion Fest! Wrap yourself in warmth with the Luxe AutumnCloud Cashmere Wrap and FrostGuard Elite Winter Parka. Enjoy up to 25% off on fall favorites. Step into the season with style! Shop now!</t>
+          <t>**Fall Fashion Fest**\tOct 01 – Oct 15\nCelebrate the beauty of autumn with our Fall Fashion Fest! Wrap yourself in warmth with the Luxe AutumnCloud Cashmere Wrap and FrostGuard Elite Winter Parka. Enjoy up to 25% off on fall favorites. Step into the season with style! Shop now!</t>
         </is>
       </c>
     </row>
@@ -819,8 +807,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>**Spring into Sound**	Mar 15 – Apr 15
-Embrace the refreshing vibes of spring with our NimbusWave Spring Breeze Portable Bluetooth Speaker. It's perfect for outdoor picnics and garden parties! Enjoy up to 15% off and elevate your music experience. Limited time offer!</t>
+          <t>**Spring into Sound**\tMar 15 – Apr 15\nEmbrace the refreshing vibes of spring with our NimbusWave Spring Breeze Portable Bluetooth Speaker. It's perfect for outdoor picnics and garden parties! Enjoy up to 15% off and elevate your music experience. Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -847,8 +834,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>**Cloudy Day Comforts**	Apr 1 – Apr 30
-Don’t let the cloudy weather dampen your spirits! Cozy up with the NimbusWave CozyHeat Radiator. Stay warm and stylish this spring with our special offer of Buy 1 Get 1 50% off. Shop now!</t>
+          <t>**Cloudy Day Comforts**\tApr 1 – Apr 30\nDon’t let the cloudy weather dampen your spirits! Cozy up with the NimbusWave CozyHeat Radiator. Stay warm and stylish this spring with our special offer of Buy 1 Get 1 50% off. Shop now!</t>
         </is>
       </c>
     </row>
@@ -875,8 +861,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>**April Showers, Great Tech**	Apr 10 – Apr 30
-Gear up for rainy days with the AquaShield Luxe Rain-Guard Charger. Keep your devices safe and powered up while enjoying spring storms. Get 10% off your purchase today! Limited stock available!</t>
+          <t>**April Showers, Great Tech**\tApr 10 – Apr 30\nGear up for rainy days with the AquaShield Luxe Rain-Guard Charger. Keep your devices safe and powered up while enjoying spring storms. Get 10% off your purchase today! Limited stock available!</t>
         </is>
       </c>
     </row>
@@ -903,8 +888,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>**Spring Sound Festival**	Mar 20 – Apr 10
-Celebrate the season of renewal with our SunnyTech BreezeGlow Portable Speaker! Enjoy vibrant sound and portability for all your spring activities. Grab yours now at 20% off! Don’t miss out!</t>
+          <t>**Spring Sound Festival**\tMar 20 – Apr 10\nCelebrate the season of renewal with our SunnyTech BreezeGlow Portable Speaker! Enjoy vibrant sound and portability for all your spring activities. Grab yours now at 20% off! Don’t miss out!</t>
         </is>
       </c>
     </row>
@@ -931,8 +915,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>**Celebrate Earth Day**	Apr 15 – Apr 25
-Go green with the FrostGuard Luxe Radiant Heater. Perfect for eco-friendly warmth this spring! Enjoy a special Earth Day discount of 15% off. Join us in celebrating sustainability! Shop now!</t>
+          <t>**Celebrate Earth Day**\tApr 15 – Apr 25\nGo green with the FrostGuard Luxe Radiant Heater. Perfect for eco-friendly warmth this spring! Enjoy a special Earth Day discount of 15% off. Join us in celebrating sustainability! Shop now!</t>
         </is>
       </c>
     </row>
@@ -959,8 +942,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>**Spring Cleaning Electronics Sale**	Mar 25 – Apr 20
-Refresh your tech collection with our Spring Cleaning Electronics Sale! Check out the NimbusCharge CloudFlex Wireless Power Bank to keep your devices charged on the go. Enjoy 10% off all items. Limited time offer!</t>
+          <t>**Spring Cleaning Electronics Sale**\tMar 25 – Apr 20\nRefresh your tech collection with our Spring Cleaning Electronics Sale! Check out the NimbusCharge CloudFlex Wireless Power Bank to keep your devices charged on the go. Enjoy 10% off all items. Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -987,8 +969,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>**Weekend Getaway Essentials**	Mar 30 – Apr 15
-Plan your spring getaway with the AutumnRain Luxe Bluetooth Earbuds for an immersive audio experience on the road. Buy 2 pairs and get 1 free! Grab this perfect travel companion now!</t>
+          <t>**Weekend Getaway Essentials**\tMar 30 – Apr 15\nPlan your spring getaway with the AutumnRain Luxe Bluetooth Earbuds for an immersive audio experience on the road. Buy 2 pairs and get 1 free! Grab this perfect travel companion now!</t>
         </is>
       </c>
     </row>
@@ -1015,8 +996,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>**Cloudy Cozy Nights**	Apr 5 – Apr 25
-Warm up your evenings with the WinterGlow Luxe Heater. Snuggle in with a good book and soft music. Get it now for a cozy discount of 20% off. Make your nights comfy!</t>
+          <t>**Cloudy Cozy Nights**\tApr 5 – Apr 25\nWarm up your evenings with the WinterGlow Luxe Heater. Snuggle in with a good book and soft music. Get it now for a cozy discount of 20% off. Make your nights comfy!</t>
         </is>
       </c>
     </row>
@@ -1043,8 +1023,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>**Spring Fling Tech Sale**	Mar 15 – Apr 30
-Fall in love with sound this spring. The SunnyWave Luxe Winter Bluetooth Speaker is perfect for all your romantic picnics. Grab yours with an exclusive 10% discount. Limited time offer!</t>
+          <t>**Spring Fling Tech Sale**\tMar 15 – Apr 30\nFall in love with sound this spring. The SunnyWave Luxe Winter Bluetooth Speaker is perfect for all your romantic picnics. Grab yours with an exclusive 10% discount. Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -1071,8 +1050,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>**Blossom into Music**	Apr 1 – Apr 15
-Let your spirit bloom with the NimbusSound CloudFlex Spring Speaker! Perfect for outdoor gatherings, now available at 15% off. Experience the joy of music in the fresh spring air. Shop now!</t>
+          <t>**Blossom into Music**\tApr 1 – Apr 15\nLet your spirit bloom with the NimbusSound CloudFlex Spring Speaker! Perfect for outdoor gatherings, now available at 15% off. Experience the joy of music in the fresh spring air. Shop now!</t>
         </is>
       </c>
     </row>
@@ -1099,8 +1077,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>**Rainy Day Fun**	Apr 10 – Apr 30
-Brighten up your rainy days with the AquaShield Summer Breeze Bluetooth Umbrella. Enjoy your favorite tunes while staying dry. Get 10% off and make every downpour a celebration! Limited stock!</t>
+          <t>**Rainy Day Fun**\tApr 10 – Apr 30\nBrighten up your rainy days with the AquaShield Summer Breeze Bluetooth Umbrella. Enjoy your favorite tunes while staying dry. Get 10% off and make every downpour a celebration! Limited stock!</t>
         </is>
       </c>
     </row>
@@ -1127,8 +1104,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>**Cozy Up for Spring**	Apr 5 – Apr 20
-Turn your home into a haven with the FrostWave Luxe Ceramic Heater. Enjoy warm vibes while the season changes. Get 15% off your purchase and embrace the cozy ambiance! Shop now!</t>
+          <t>**Cozy Up for Spring**\tApr 5 – Apr 20\nTurn your home into a haven with the FrostWave Luxe Ceramic Heater. Enjoy warm vibes while the season changes. Get 15% off your purchase and embrace the cozy ambiance! Shop now!</t>
         </is>
       </c>
     </row>
@@ -1155,8 +1131,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>**Spring Refresh Sale**	Mar 15 – Apr 15
-Embrace the beauty of spring with our Spring Refresh Sale! Transform your space with the LuxeRain Spring Patio Lounge Chair and SunnyNest Coastal Charm Accent Table. Enjoy a cozy atmosphere with up to 15% off selected items. Breathe new life into your home this season! Shop now!</t>
+          <t>**Spring Refresh Sale**\tMar 15 – Apr 15\nEmbrace the beauty of spring with our Spring Refresh Sale! Transform your space with the LuxeRain Spring Patio Lounge Chair and SunnyNest Coastal Charm Accent Table. Enjoy a cozy atmosphere with up to 15% off selected items. Breathe new life into your home this season! Shop now!</t>
         </is>
       </c>
     </row>
@@ -1183,8 +1158,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>**Rainy Day Comfort**	Apr 01 – Apr 30
-Don’t let the rain dampen your spirits! Snuggle up with our NimbusNest Luxe Cloud Lounge Chair and AutumnRain Luxe Armchair. Enjoy a special offer of Buy 1 Get 1 at 20% off! Create a cozy retreat that makes every rainy day feel like a cozy escape. Limited time offer!</t>
+          <t>**Rainy Day Comfort**\tApr 01 – Apr 30\nDon’t let the rain dampen your spirits! Snuggle up with our NimbusNest Luxe Cloud Lounge Chair and AutumnRain Luxe Armchair. Enjoy a special offer of Buy 1 Get 1 at 20% off! Create a cozy retreat that makes every rainy day feel like a cozy escape. Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -1211,8 +1185,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>**Spring Fling Furniture Fest**	Apr 10 – Apr 25
-Celebrate spring with our Spring Fling Furniture Fest! Discover the chic AutumnLuxe Maple Accent Chair and the refreshing LuxeCloud Springtime Lounge Chair. Enjoy up to 25% off on select pieces! Revitalize your home and let the sunshine in! Shop now!</t>
+          <t>**Spring Fling Furniture Fest**\tApr 10 – Apr 25\nCelebrate spring with our Spring Fling Furniture Fest! Discover the chic AutumnLuxe Maple Accent Chair and the refreshing LuxeCloud Springtime Lounge Chair. Enjoy up to 25% off on select pieces! Revitalize your home and let the sunshine in! Shop now!</t>
         </is>
       </c>
     </row>
@@ -1239,8 +1212,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>**Easter Home Makeover**	Mar 20 – Apr 10
-Hop into our Easter Home Makeover with delightful discounts! Brighten your living space with the Frosted Birch WinterGlow Accent Table or the AmberGlow Autumn Lounge Chair. Get up to 20% off storewide and create a space that welcomes spring! Limited time offer!</t>
+          <t>**Easter Home Makeover**\tMar 20 – Apr 10\nHop into our Easter Home Makeover with delightful discounts! Brighten your living space with the Frosted Birch WinterGlow Accent Table or the AmberGlow Autumn Lounge Chair. Get up to 20% off storewide and create a space that welcomes spring! Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -1267,8 +1239,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>**Monsoon Magic Sale**	Jun 01 – Jun 15
-Experience the magic of monsoon with our exclusive Monsoon Magic Sale! Discover the rain-resistant Autumn Luxe Rain-Resistant Accent Chair and Luxe RainySpring Chair at up to 30% off. Perfect for cozy evenings and afternoon reads. Don’t miss out—shop now!</t>
+          <t>**Monsoon Magic Sale**\tJun 01 – Jun 15\nExperience the magic of monsoon with our exclusive Monsoon Magic Sale! Discover the rain-resistant Autumn Luxe Rain-Resistant Accent Chair and Luxe RainySpring Chair at up to 30% off. Perfect for cozy evenings and afternoon reads. Don’t miss out—shop now!</t>
         </is>
       </c>
     </row>
@@ -1295,8 +1266,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>**Coastal Charm Week**	May 01 – May 07
-Dive into summer vibes with our Coastal Charm Week! Celebrate with the SunnyNest Coastal Charm Accent Table and the SunnyNest Luxe Summer Lounge Chair. Enjoy an enticing Buy 2 Get 1 Free offer on all accent tables! Refresh your home with coastal flair!</t>
+          <t>**Coastal Charm Week**\tMay 01 – May 07\nDive into summer vibes with our Coastal Charm Week! Celebrate with the SunnyNest Coastal Charm Accent Table and the SunnyNest Luxe Summer Lounge Chair. Enjoy an enticing Buy 2 Get 1 Free offer on all accent tables! Refresh your home with coastal flair!</t>
         </is>
       </c>
     </row>
@@ -1323,8 +1293,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>**Spring into Savings**	Apr 20 – May 20
-It’s the season of renewal! Spring into savings with the NimbusNest Cloud Comfort Chair and Luxe Frosted Maple Side Table. Enjoy up to 20% off select furniture pieces to create your ideal spring sanctuary. Shop now and elevate your space!</t>
+          <t>**Spring into Savings**\tApr 20 – May 20\nIt’s the season of renewal! Spring into savings with the NimbusNest Cloud Comfort Chair and Luxe Frosted Maple Side Table. Enjoy up to 20% off select furniture pieces to create your ideal spring sanctuary. Shop now and elevate your space!</t>
         </is>
       </c>
     </row>
@@ -1351,8 +1320,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>**Rainy Day Retreat**	Jul 01 – Jul 15
-Create your rainy day retreat with our special collection! Snuggle up on the NimbusNest Luxe Cloud Lounge Chair and add the AutumnGlow Rustic Side Table to complete your cozy corner. Enjoy up to 15% off on select lounge chairs! Limited time offer!</t>
+          <t>**Rainy Day Retreat**\tJul 01 – Jul 15\nCreate your rainy day retreat with our special collection! Snuggle up on the NimbusNest Luxe Cloud Lounge Chair and add the AutumnGlow Rustic Side Table to complete your cozy corner. Enjoy up to 15% off on select lounge chairs! Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -1379,8 +1347,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>**Summer Splash Sale**	Jun 20 – Jul 05
-Make a splash this summer with our Summer Splash Sale! Get the SunnyNest Luxe Summer Lounge Chair and the AmberGlow Autumn Lounge Chair at fabulous discounts of up to 25%! Perfect for those sunny days! Don’t wait—shop now!</t>
+          <t>**Summer Splash Sale**\tJun 20 – Jul 05\nMake a splash this summer with our Summer Splash Sale! Get the SunnyNest Luxe Summer Lounge Chair and the AmberGlow Autumn Lounge Chair at fabulous discounts of up to 25%! Perfect for those sunny days! Don’t wait—shop now!</t>
         </is>
       </c>
     </row>
@@ -1407,8 +1374,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>**Spring Clean &amp; Style**	Mar 01 – Mar 31
-Refresh your home this spring with our Spring Clean &amp; Style campaign! Uncover stylish finds like the LuxeCloud Springtime Lounge Chair and the Frosted Birch WinterGlow Accent Table. Enjoy a special 15% discount on select items! Give your space a fresh look!</t>
+          <t>**Spring Clean &amp; Style**\tMar 01 – Mar 31\nRefresh your home this spring with our Spring Clean &amp; Style campaign! Uncover stylish finds like the LuxeCloud Springtime Lounge Chair and the Frosted Birch WinterGlow Accent Table. Enjoy a special 15% discount on select items! Give your space a fresh look!</t>
         </is>
       </c>
     </row>
@@ -1435,8 +1401,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>**Furniture Festival Extravaganza**	Apr 15 – May 05
-Join our Furniture Festival Extravaganza and elevate your home decor! Explore the AmberGlow Autumn Lounge Chair and Luxe RainySpring Chair with up to 20% off storewide! Perfect for indoor relaxation or outdoor enjoyment. Limited time offer—shop now!</t>
+          <t>**Furniture Festival Extravaganza**\tApr 15 – May 05\nJoin our Furniture Festival Extravaganza and elevate your home decor! Explore the AmberGlow Autumn Lounge Chair and Luxe RainySpring Chair with up to 20% off storewide! Perfect for indoor relaxation or outdoor enjoyment. Limited time offer—shop now!</t>
         </is>
       </c>
     </row>
@@ -1463,8 +1428,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>**End of Spring Sale**	May 15 – May 31
-Celebrate the end of spring with our exclusive sale! Discover the AutumnLuxe Maple Accent Chair and the LuxeRain Spring Patio Lounge Chair at up to 30% off. Perfect for making the most of the season before summer! Don’t miss out—shop today!</t>
+          <t>**End of Spring Sale**\tMay 15 – May 31\nCelebrate the end of spring with our exclusive sale! Discover the AutumnLuxe Maple Accent Chair and the LuxeRain Spring Patio Lounge Chair at up to 30% off. Perfect for making the most of the season before summer! Don’t miss out—shop today!</t>
         </is>
       </c>
     </row>
@@ -1491,8 +1455,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>**Autumn Harvest Festival**	Oct 01 – Oct 31
-Celebrate the bounty of the season with our Autumn Harvest Festival! Enjoy the rich flavors of our HarvestGlow Autumn Spice Blend and indulge in the comforting taste of FrostHarvest Gourmet Soup Medley. Enjoy up to 15% off select products. Cozy up with these seasonal delights! Shop now!</t>
+          <t>**Autumn Harvest Festival**\tOct 01 – Oct 31\nCelebrate the bounty of the season with our Autumn Harvest Festival! Enjoy the rich flavors of our HarvestGlow Autumn Spice Blend and indulge in the comforting taste of FrostHarvest Gourmet Soup Medley. Enjoy up to 15% off select products. Cozy up with these seasonal delights! Shop now!</t>
         </is>
       </c>
     </row>
@@ -1519,8 +1482,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>**Snowy Comforts Sale**	Nov 15 – Dec 05
-As the snow begins to fall, warm your heart and home with our Snowy Comforts Sale! Discover the warm embrace of FrostyHarvest Seasonal Comfort Soup Mix and our HarvestEssence Spiced Pumpkin Velvet Soup. Enjoy Buy 2 Get 1 Free on all soups. Limited time offer!</t>
+          <t>**Snowy Comforts Sale**\tNov 15 – Dec 05\nAs the snow begins to fall, warm your heart and home with our Snowy Comforts Sale! Discover the warm embrace of FrostyHarvest Seasonal Comfort Soup Mix and our HarvestEssence Spiced Pumpkin Velvet Soup. Enjoy Buy 2 Get 1 Free on all soups. Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -1547,8 +1509,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>**Citrus Delight Week**	Dec 10 – Dec 17
-Brighten your winter days with our Citrus Delight Week! Refresh your senses with SunnyHarvest Citrus Splash Infusion and Citrus Frosted Bliss Bites. Enjoy up to 20% off all citrus products. Add a splash of sunshine to your grocery list! Shop now!</t>
+          <t>**Citrus Delight Week**\tDec 10 – Dec 17\nBrighten your winter days with our Citrus Delight Week! Refresh your senses with SunnyHarvest Citrus Splash Infusion and Citrus Frosted Bliss Bites. Enjoy up to 20% off all citrus products. Add a splash of sunshine to your grocery list! Shop now!</t>
         </is>
       </c>
     </row>
@@ -1575,8 +1536,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>**Harvest Your Favorites**	Oct 15 – Nov 15
-Dive into the flavors of fall with our Harvest Your Favorites promotion! Savor the taste of AutumnHarvest Crisp Apples and FrostyHarvest Summer Berry Medley. Enjoy 10% off when you mix and match your favorite harvest snacks. Taste the season today!</t>
+          <t>**Harvest Your Favorites**\tOct 15 – Nov 15\nDive into the flavors of fall with our Harvest Your Favorites promotion! Savor the taste of AutumnHarvest Crisp Apples and FrostyHarvest Summer Berry Medley. Enjoy 10% off when you mix and match your favorite harvest snacks. Taste the season today!</t>
         </is>
       </c>
     </row>
@@ -1603,8 +1563,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>**Cozy Soup Sundays**	Nov 01 – Nov 30
-This November, turn Sundays into cozy soup days! With our FrostyHarvest Artisan Soup Mix and RainyDay Gourmet Soup Blend, your family will love the warmth of homemade flavors. Enjoy up to 25% off on all soups every Sunday. Grab yours now!</t>
+          <t>**Cozy Soup Sundays**\tNov 01 – Nov 30\nThis November, turn Sundays into cozy soup days! With our FrostyHarvest Artisan Soup Mix and RainyDay Gourmet Soup Blend, your family will love the warmth of homemade flavors. Enjoy up to 25% off on all soups every Sunday. Grab yours now!</t>
         </is>
       </c>
     </row>
@@ -1631,8 +1590,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>**Frosty Delights Celebration**	Dec 01 – Dec 20
-Embrace the frosty season with our Frosty Delights Celebration! Treat yourself to FrostyHarvest Summer Citrus Splash and SunnyHarvest Tropical Bliss Fruit Medley. Enjoy 15% off on all frosty products. Don’t miss out on the fun—shop today!</t>
+          <t>**Frosty Delights Celebration**\tDec 01 – Dec 20\nEmbrace the frosty season with our Frosty Delights Celebration! Treat yourself to FrostyHarvest Summer Citrus Splash and SunnyHarvest Tropical Bliss Fruit Medley. Enjoy 15% off on all frosty products. Don’t miss out on the fun—shop today!</t>
         </is>
       </c>
     </row>
@@ -1659,8 +1617,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>**Thanksgiving Feast Essentials**	Nov 20 – Nov 25
-Prepare for a Thanksgiving feast with our essential grocery items! Stock up on HarvestEssence Summer Cloudberry Delight and HarvestNest Spring Essence Organic Quinoa for a delightful twist to your holiday table. Enjoy up to 10% off on select products. Celebrate with flavor!</t>
+          <t>**Thanksgiving Feast Essentials**\tNov 20 – Nov 25\nPrepare for a Thanksgiving feast with our essential grocery items! Stock up on HarvestEssence Summer Cloudberry Delight and HarvestNest Spring Essence Organic Quinoa for a delightful twist to your holiday table. Enjoy up to 10% off on select products. Celebrate with flavor!</t>
         </is>
       </c>
     </row>
@@ -1687,8 +1644,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>**Winter Wellness Week**	Dec 05 – Dec 12
-Keep your family healthy this winter with our Winter Wellness Week! Enjoy the nourishing benefits of FrostHarvest Gourmet Soup Medley and SunnyHarvest Citrus Refresh. Get 20% off on select health-focused groceries. Stay well and shop now!</t>
+          <t>**Winter Wellness Week**\tDec 05 – Dec 12\nKeep your family healthy this winter with our Winter Wellness Week! Enjoy the nourishing benefits of FrostHarvest Gourmet Soup Medley and SunnyHarvest Citrus Refresh. Get 20% off on select health-focused groceries. Stay well and shop now!</t>
         </is>
       </c>
     </row>
@@ -1715,8 +1671,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>**Season’s Greetings Special**	Dec 15 – Dec 31
-Spread joy this holiday season with our Season’s Greetings Special! Delight in the taste of HarvestGlow Autumn Spice Blend and FrostyHarvest Summer Berry Medley. Enjoy Buy 1 Get 1 50% off on festive favorites. Limited time offer!</t>
+          <t>**Season’s Greetings Special**\tDec 15 – Dec 31\nSpread joy this holiday season with our Season’s Greetings Special! Delight in the taste of HarvestGlow Autumn Spice Blend and FrostyHarvest Summer Berry Medley. Enjoy Buy 1 Get 1 50% off on festive favorites. Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -1743,8 +1698,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>**New Year Fresh Start**	Jan 01 – Jan 15
-Kickstart your New Year with a fresh start! Stock your pantry with HarvestNest Spring Essence Organic Quinoa and SunnyHarvest Tropical Bliss Fruit Medley. Enjoy 15% off on all health-conscious groceries. Start the year right—shop now!</t>
+          <t>**New Year Fresh Start**\tJan 01 – Jan 15\nKickstart your New Year with a fresh start! Stock your pantry with HarvestNest Spring Essence Organic Quinoa and SunnyHarvest Tropical Bliss Fruit Medley. Enjoy 15% off on all health-conscious groceries. Start the year right—shop now!</t>
         </is>
       </c>
     </row>
@@ -1771,8 +1725,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>**Savor the Season Sale**	Oct 25 – Nov 10
-Savor the flavors of autumn with our Savor the Season Sale! Discover the deliciousness of FrostyHarvest Seasonal Comfort Soup Mix and AutumnHarvest Crisp Apples. Enjoy 10% off select products. Immerse yourself in the season’s best—shop today!</t>
+          <t>**Savor the Season Sale**\tOct 25 – Nov 10\nSavor the flavors of autumn with our Savor the Season Sale! Discover the deliciousness of FrostyHarvest Seasonal Comfort Soup Mix and AutumnHarvest Crisp Apples. Enjoy 10% off select products. Immerse yourself in the season’s best—shop today!</t>
         </is>
       </c>
     </row>
@@ -1799,8 +1752,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>**Chilly Days, Cozy Nights**	Nov 10 – Nov 30
-Embrace chilly days with warm, hearty meals! Enjoy the comforting warmth of FrostyHarvest Artisan Soup Mix and HarvestEssence Spiced Pumpkin Velvet Soup. Enjoy up to 20% off on all cozy products. Make your evenings special—grab yours now!</t>
+          <t>**Chilly Days, Cozy Nights**\tNov 10 – Nov 30\nEmbrace chilly days with warm, hearty meals! Enjoy the comforting warmth of FrostyHarvest Artisan Soup Mix and HarvestEssence Spiced Pumpkin Velvet Soup. Enjoy up to 20% off on all cozy products. Make your evenings special—grab yours now!</t>
         </is>
       </c>
     </row>
@@ -1827,8 +1779,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>**Winter Wonderland Magic**	Dec 1 – Dec 25
-Embrace the snowy season with our CozyHaven Winter Wonderland Playhouse! Let your children's imaginations soar as they build their own winter retreat. Enjoy up to 15% off on all winter toys. Create magical memories this holiday season! Shop now!</t>
+          <t>**Winter Wonderland Magic**\tDec 1 – Dec 25\nEmbrace the snowy season with our CozyHaven Winter Wonderland Playhouse! Let your children's imaginations soar as they build their own winter retreat. Enjoy up to 15% off on all winter toys. Create magical memories this holiday season! Shop now!</t>
         </is>
       </c>
     </row>
@@ -1855,8 +1806,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>**Sledding Into Fun**	Dec 15 – Jan 5
-Experience the thrill of winter sledding with our Snowy Luxe Plush Sledding Toy! Perfect for cozy winter days, this plush companion makes every snow adventure delightful. Grab yours with a special offer of Buy 2 Get 1 Free! Limited time offer!</t>
+          <t>**Sledding Into Fun**\tDec 15 – Jan 5\nExperience the thrill of winter sledding with our Snowy Luxe Plush Sledding Toy! Perfect for cozy winter days, this plush companion makes every snow adventure delightful. Grab yours with a special offer of Buy 2 Get 1 Free! Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -1883,8 +1833,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>**Frosty Fun Fest**	Dec 20 – Jan 10
-Get ready for winter fun with the FrostyPlay Deluxe Snowball Maker! Make snowballs in seconds and turn your backyard into a snowy playground. For a limited time, enjoy up to 20% off on all snow-themed toys. Don't miss out!</t>
+          <t>**Frosty Fun Fest**\tDec 20 – Jan 10\nGet ready for winter fun with the FrostyPlay Deluxe Snowball Maker! Make snowballs in seconds and turn your backyard into a snowy playground. For a limited time, enjoy up to 20% off on all snow-themed toys. Don't miss out!</t>
         </is>
       </c>
     </row>
@@ -1911,8 +1860,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>**Holiday Adventure Kit**	Dec 10 – Dec 24
-Equip your little explorers with the SunnyQuest Adventure Explorer Backpack! Perfect for winter hikes or snowy adventures, it's packed with everything they need for fun. Enjoy up to 10% off this festive season! Shop now and explore!</t>
+          <t>**Holiday Adventure Kit**\tDec 10 – Dec 24\nEquip your little explorers with the SunnyQuest Adventure Explorer Backpack! Perfect for winter hikes or snowy adventures, it's packed with everything they need for fun. Enjoy up to 10% off this festive season! Shop now and explore!</t>
         </is>
       </c>
     </row>
@@ -1939,8 +1887,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>**Winter Games Extravaganza**	Dec 26 – Jan 15
-Celebrate the winter season with our WinterGlow Snowfall Playset! Create your own frosty world and engage in endless imaginative play. Buy 2 toys and get 1 free! Bring the magic of winter home today!</t>
+          <t>**Winter Games Extravaganza**\tDec 26 – Jan 15\nCelebrate the winter season with our WinterGlow Snowfall Playset! Create your own frosty world and engage in endless imaginative play. Buy 2 toys and get 1 free! Bring the magic of winter home today!</t>
         </is>
       </c>
     </row>
@@ -1967,8 +1914,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>**New Year, New Adventures**	Jan 1 – Jan 20
-Kick off the new year with the SpringCloud Adventure Kit! Inspire creativity and adventure in your little ones this winter with our engaging playsets. Enjoy an exclusive 15% off all kits for a limited time! Limited time offer!</t>
+          <t>**New Year, New Adventures**\tJan 1 – Jan 20\nKick off the new year with the SpringCloud Adventure Kit! Inspire creativity and adventure in your little ones this winter with our engaging playsets. Enjoy an exclusive 15% off all kits for a limited time! Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -1995,8 +1941,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>**Kite in the Snow**	Jan 5 – Jan 25
-Who says kites are just for summer? Introduce the NimbusPlay CloudGlide Kite to your winter fun! Watch it dance in the chilly breeze. Get yours now and enjoy up to 10% off on all kites. Shop now!</t>
+          <t>**Kite in the Snow**\tJan 5 – Jan 25\nWho says kites are just for summer? Introduce the NimbusPlay CloudGlide Kite to your winter fun! Watch it dance in the chilly breeze. Get yours now and enjoy up to 10% off on all kites. Shop now!</t>
         </is>
       </c>
     </row>
@@ -2023,8 +1968,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>**Cozy Up with Play**	Jan 15 – Feb 5
-Snuggle into winter with our SunnyWhims Winter Enchanted Castle Playset! Let your children build their own magical kingdom right at home. Enjoy a special offer of up to 15% off on all playsets this chilly season! Limited time offer!</t>
+          <t>**Cozy Up with Play**\tJan 15 – Feb 5\nSnuggle into winter with our SunnyWhims Winter Enchanted Castle Playset! Let your children build their own magical kingdom right at home. Enjoy a special offer of up to 15% off on all playsets this chilly season! Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -2051,8 +1995,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>**Winter Adventure Awaits**	Jan 10 – Jan 30
-Equip your kids for snowy escapades with the SunnyGlow Winter Wonderland Adventure Kit! Packed with exciting activities, it’s perfect for indoor and outdoor fun. Enjoy up to 10% off this winter! Shop now!</t>
+          <t>**Winter Adventure Awaits**\tJan 10 – Jan 30\nEquip your kids for snowy escapades with the SunnyGlow Winter Wonderland Adventure Kit! Packed with exciting activities, it’s perfect for indoor and outdoor fun. Enjoy up to 10% off this winter! Shop now!</t>
         </is>
       </c>
     </row>
@@ -2079,8 +2022,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>**Raindrop Wonderland**	Jan 25 – Feb 15
-Bring the magic of winter indoors with our Raindrop Luxe Playset! This captivating playset offers imaginative adventures all season long. Take advantage of our special offer: Buy 2 Get 1 Free on all playsets! Limited time offer!</t>
+          <t>**Raindrop Wonderland**\tJan 25 – Feb 15\nBring the magic of winter indoors with our Raindrop Luxe Playset! This captivating playset offers imaginative adventures all season long. Take advantage of our special offer: Buy 2 Get 1 Free on all playsets! Limited time offer!</t>
         </is>
       </c>
     </row>
@@ -2107,8 +2049,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>**Sunny Harvest Sale**	Feb 1 – Feb 20
-Brighten up the winter gloom with the SunnyHarvest Luxe Adventure Kite! Perfect for those clear winter skies, it’s time to let your child's imagination take flight. Enjoy up to 15% off on all kites this season! Shop now!</t>
+          <t>**Sunny Harvest Sale**\tFeb 1 – Feb 20\nBrighten up the winter gloom with the SunnyHarvest Luxe Adventure Kite! Perfect for those clear winter skies, it’s time to let your child's imagination take flight. Enjoy up to 15% off on all kites this season! Shop now!</t>
         </is>
       </c>
     </row>
@@ -2135,8 +2076,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>**End	of-Winter Clearance** – Feb 15 – Feb 28
-Celebrate the end of winter with a fantastic clearance sale! Get amazing discounts on all winter toys including the CloudPlay Adventure Splash Kit and more. Enjoy up to 25% off while supplies last! Don't miss out!</t>
+          <t>**End\tof-Winter Clearance** – Feb 15 – Feb 28\nCelebrate the end of winter with a fantastic clearance sale! Get amazing discounts on all winter toys including the CloudPlay Adventure Splash Kit and more. Enjoy up to 25% off while supplies last! Don't miss out!</t>
         </is>
       </c>
     </row>

</xml_diff>